<commit_message>
Added verify defined asset ownership
</commit_message>
<xml_diff>
--- a/Vulnerability-Management-Levels.xlsx
+++ b/Vulnerability-Management-Levels.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1037" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="398">
   <si>
     <t>ASVS Item #</t>
   </si>
@@ -1221,6 +1221,9 @@
   </si>
   <si>
     <t>8. Documentation/Metrics</t>
+  </si>
+  <si>
+    <t>Verify defined asset ownership standard exists</t>
   </si>
 </sst>
 </file>
@@ -4532,10 +4535,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4668,25 +4671,25 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>356</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>357</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>358</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>9</v>
@@ -4700,7 +4703,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>9</v>
@@ -4714,7 +4717,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>9</v>
@@ -4728,7 +4731,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>9</v>
@@ -4742,10 +4745,10 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>9</v>
@@ -4756,24 +4759,21 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
+        <v>362</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
         <v>363</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>376</v>
-      </c>
-      <c r="B16" t="s">
-        <v>377</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>9</v>
@@ -4787,58 +4787,61 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>376</v>
+      </c>
+      <c r="B17" t="s">
+        <v>377</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>378</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>379</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+      <c r="C18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
         <v>380</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="C19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>393</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>364</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>365</v>
-      </c>
       <c r="C20" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>9</v>
@@ -4849,13 +4852,13 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>9</v>
@@ -4863,13 +4866,13 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>9</v>
@@ -4877,10 +4880,10 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>9</v>
@@ -4891,38 +4894,38 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
+        <v>368</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
         <v>369</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="C25" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>394</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>374</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>372</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>16</v>
@@ -4936,13 +4939,13 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>9</v>
@@ -4950,13 +4953,13 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>9</v>
@@ -4964,7 +4967,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>370</v>
+        <v>375</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>16</v>
@@ -4978,38 +4981,38 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
+        <v>370</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
         <v>371</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="C31" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>395</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>381</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>382</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>16</v>
@@ -5023,7 +5026,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>16</v>
@@ -5037,13 +5040,13 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>9</v>
@@ -5051,13 +5054,13 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>9</v>
@@ -5065,7 +5068,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>345</v>
+        <v>385</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>16</v>
@@ -5079,38 +5082,38 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
+        <v>345</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
         <v>392</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="C38" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>396</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>386</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>349</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>16</v>
@@ -5124,7 +5127,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>387</v>
+        <v>349</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>16</v>
@@ -5138,7 +5141,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>16</v>
@@ -5152,7 +5155,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>16</v>
@@ -5166,7 +5169,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>350</v>
+        <v>389</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>16</v>
@@ -5180,13 +5183,13 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>390</v>
+        <v>350</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>9</v>
@@ -5194,15 +5197,29 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
+        <v>390</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
         <v>391</v>
       </c>
-      <c r="C45" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E45" s="1" t="s">
+      <c r="C46" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E46" s="1" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>